<commit_message>
Add cad_icon via svg
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Оценка</t>
   </si>
@@ -55,13 +55,34 @@
   </si>
   <si>
     <t>Возможно стоит разместить запрос по поводу drag компонента</t>
+  </si>
+  <si>
+    <t>Настроить VS Code, tabs, indentation and formatting</t>
+  </si>
+  <si>
+    <t>Разработать иконки для следующих примитивов:</t>
+  </si>
+  <si>
+    <t>прямоугольник</t>
+  </si>
+  <si>
+    <t>круг</t>
+  </si>
+  <si>
+    <t>текстовое поле</t>
+  </si>
+  <si>
+    <t>кривая</t>
+  </si>
+  <si>
+    <t>ломаная линия</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +105,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -118,7 +146,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -138,6 +166,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Нейтральный" xfId="2" builtinId="28"/>
@@ -420,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +514,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -501,7 +533,7 @@
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -510,14 +542,55 @@
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.4">
+      <c r="B9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>